<commit_message>
spi implemented, adc corrected, some pins/ports corrected, cj125 basic communication implemented
</commit_message>
<xml_diff>
--- a/hardware/Datasheet/berechnungen.xlsx
+++ b/hardware/Datasheet/berechnungen.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="PWM" sheetId="1" r:id="rId1"/>
+    <sheet name="ADC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Fcpu</t>
   </si>
@@ -34,6 +35,27 @@
   </si>
   <si>
     <t>TOP</t>
+  </si>
+  <si>
+    <t>Referenz, V</t>
+  </si>
+  <si>
+    <t>ADC Wert</t>
+  </si>
+  <si>
+    <t>ADC-Spannung, V</t>
+  </si>
+  <si>
+    <t>Spannungsteiler</t>
+  </si>
+  <si>
+    <t>echte Spannung, V</t>
+  </si>
+  <si>
+    <t>Gesamtwiderstand / Massenwiderstand</t>
+  </si>
+  <si>
+    <t>ADC-Wert</t>
   </si>
 </sst>
 </file>
@@ -398,4 +420,97 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>543</v>
+      </c>
+      <c r="C2">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <f>B2*(B1/1024)</f>
+        <v>2.6513671875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <f>B3*B4</f>
+        <v>12.991699218750002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <f>B9/B4</f>
+        <v>2.6530612244897958</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <f>(B10*1024)/5</f>
+        <v>543.34693877551013</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adc input reading corrected
</commit_message>
<xml_diff>
--- a/hardware/Datasheet/berechnungen.xlsx
+++ b/hardware/Datasheet/berechnungen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PWM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Fcpu</t>
   </si>
@@ -56,6 +56,21 @@
   </si>
   <si>
     <t>ADC-Wert</t>
+  </si>
+  <si>
+    <t>Resolution, bit</t>
+  </si>
+  <si>
+    <t>Ubat, V</t>
+  </si>
+  <si>
+    <t>condens, V</t>
+  </si>
+  <si>
+    <t>duty, %</t>
+  </si>
+  <si>
+    <t>dutyCycle</t>
   </si>
 </sst>
 </file>
@@ -373,13 +388,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -402,19 +420,62 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>1023</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>POWER(2,10)-1</f>
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <f>B1/(B2*(1+B3))</f>
+      <c r="B5">
+        <f>B1/(B2*(1+B4))</f>
         <v>244.140625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <f>(B9/B8)*100</f>
+        <v>11.029411764705882</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <f>(1024*B10)/100</f>
+        <v>112.94117647058823</v>
       </c>
     </row>
   </sheetData>
@@ -426,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -449,7 +510,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>543</v>
+        <v>563</v>
       </c>
       <c r="C2">
         <v>566</v>
@@ -461,7 +522,7 @@
       </c>
       <c r="B3">
         <f>B2*(B1/1024)</f>
-        <v>2.6513671875</v>
+        <v>2.7490234375</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -481,7 +542,7 @@
       </c>
       <c r="B5">
         <f>B3*B4</f>
-        <v>12.991699218750002</v>
+        <v>13.470214843750002</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
-> new datasheet added -> start pwm duty set to 0 -> lsu 4.9 pin out added
</commit_message>
<xml_diff>
--- a/hardware/Datasheet/berechnungen.xlsx
+++ b/hardware/Datasheet/berechnungen.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PWM" sheetId="1" r:id="rId1"/>
     <sheet name="ADC" sheetId="2" r:id="rId2"/>
+    <sheet name="LSU 4.9 Pinout" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Fcpu</t>
   </si>
@@ -71,14 +72,88 @@
   </si>
   <si>
     <t>dutyCycle</t>
+  </si>
+  <si>
+    <t>Pin#</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>grey</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>VM</t>
+  </si>
+  <si>
+    <t>Uh-</t>
+  </si>
+  <si>
+    <t>Uh+</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>Pump current APE</t>
+  </si>
+  <si>
+    <t>Virtual groun</t>
+  </si>
+  <si>
+    <t>Heater voltage H+</t>
+  </si>
+  <si>
+    <t>Heater voltage H-</t>
+  </si>
+  <si>
+    <t>Trim resistor</t>
+  </si>
+  <si>
+    <t>Nernst voltage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -106,8 +181,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -123,6 +199,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>649329</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95953</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="1533525"/>
+          <a:ext cx="11669754" cy="5039428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -487,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -574,4 +693,123 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>